<commit_message>
conduct S1 tests for REST and GraphQL
</commit_message>
<xml_diff>
--- a/Wyniki/S1-GraphQL.xlsx
+++ b/Wyniki/S1-GraphQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD2F057-C400-47A5-AB08-10FB37ED5E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964BB24A-1FFA-4925-AC17-0D8133CC4898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 wiersz" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="75">
   <si>
     <t>Maksymalna liczba użytkowników</t>
   </si>
@@ -68,114 +68,15 @@
     <t>p(95) (ms)</t>
   </si>
   <si>
-    <t>403,1 µs</t>
-  </si>
-  <si>
     <t>Otrzymane dane (GB)</t>
   </si>
   <si>
-    <t>354,9 µs</t>
-  </si>
-  <si>
-    <t>325,29 µs</t>
-  </si>
-  <si>
-    <t>314,2 µs</t>
-  </si>
-  <si>
-    <t>329 µs</t>
-  </si>
-  <si>
-    <t>457,1 µs</t>
-  </si>
-  <si>
-    <t>400,9 µs</t>
-  </si>
-  <si>
-    <t>502,49 µs</t>
-  </si>
-  <si>
-    <t>349,3 µs</t>
-  </si>
-  <si>
-    <t>414,9 µs</t>
-  </si>
-  <si>
-    <t>502,9 µs</t>
-  </si>
-  <si>
     <t>508,1 µs</t>
   </si>
   <si>
-    <t>511 µs</t>
-  </si>
-  <si>
-    <t>507,7  µs</t>
-  </si>
-  <si>
-    <t>513,29 µs</t>
-  </si>
-  <si>
     <t>504,2 µs</t>
   </si>
   <si>
-    <t>503,8 µs</t>
-  </si>
-  <si>
-    <t>309,9 µs</t>
-  </si>
-  <si>
-    <t>502,29 µs</t>
-  </si>
-  <si>
-    <t>505 µs</t>
-  </si>
-  <si>
-    <t>503,1 µs</t>
-  </si>
-  <si>
-    <t>321,4 µs</t>
-  </si>
-  <si>
-    <t>461,4 µs</t>
-  </si>
-  <si>
-    <t>466,7 µs</t>
-  </si>
-  <si>
-    <t>502,7 µs</t>
-  </si>
-  <si>
-    <t>505,2 µs</t>
-  </si>
-  <si>
-    <t>502,8 µs</t>
-  </si>
-  <si>
-    <t>505,6 µs</t>
-  </si>
-  <si>
-    <t>436,3 µs</t>
-  </si>
-  <si>
-    <t>504,29 µs</t>
-  </si>
-  <si>
-    <t>503,4 µs</t>
-  </si>
-  <si>
-    <t>507,2 µs</t>
-  </si>
-  <si>
-    <t>506,8 µs</t>
-  </si>
-  <si>
-    <t>504,9 µs</t>
-  </si>
-  <si>
-    <t>507 µs</t>
-  </si>
-  <si>
     <t>993,27µs</t>
   </si>
   <si>
@@ -267,6 +168,90 @@
   </si>
   <si>
     <t>505,9µs</t>
+  </si>
+  <si>
+    <t>521,59 µs</t>
+  </si>
+  <si>
+    <t>525,69 µs</t>
+  </si>
+  <si>
+    <t>36,,18</t>
+  </si>
+  <si>
+    <t>482,5 µs</t>
+  </si>
+  <si>
+    <t>508,2 µs</t>
+  </si>
+  <si>
+    <t>48.7</t>
+  </si>
+  <si>
+    <t>508.2µs</t>
+  </si>
+  <si>
+    <t>77.84</t>
+  </si>
+  <si>
+    <t>86.25</t>
+  </si>
+  <si>
+    <t>23.47</t>
+  </si>
+  <si>
+    <t>509.1µs</t>
+  </si>
+  <si>
+    <t>18.59</t>
+  </si>
+  <si>
+    <t>495.9µs</t>
+  </si>
+  <si>
+    <t>235.54</t>
+  </si>
+  <si>
+    <t>19.41</t>
+  </si>
+  <si>
+    <t>511.1µs</t>
+  </si>
+  <si>
+    <t>528,59 µs</t>
+  </si>
+  <si>
+    <t>519,5 µs</t>
+  </si>
+  <si>
+    <t>527,9 µs</t>
+  </si>
+  <si>
+    <t>522,8 µs</t>
+  </si>
+  <si>
+    <t>506,1 µs</t>
+  </si>
+  <si>
+    <t>569,9 µs</t>
+  </si>
+  <si>
+    <t>616 µs</t>
+  </si>
+  <si>
+    <t>517,9 µs</t>
+  </si>
+  <si>
+    <t>652.59µs</t>
+  </si>
+  <si>
+    <t>19h</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>14,4h</t>
   </si>
 </sst>
 </file>
@@ -282,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,8 +286,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -325,11 +316,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -340,13 +355,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -631,36 +658,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E2:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="33" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="11" width="10.7265625" customWidth="1"/>
+    <col min="7" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="5:17" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="5:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="5:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,8 +728,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E5" s="5">
+    <row r="5" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E5" s="8">
         <v>100</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -730,8 +757,8 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E6" s="5"/>
+    <row r="6" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E6" s="8"/>
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
@@ -757,8 +784,8 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E7" s="5"/>
+    <row r="7" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E7" s="8"/>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
@@ -784,8 +811,8 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E8" s="5"/>
+    <row r="8" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E8" s="8"/>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -811,8 +838,8 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E9" s="5"/>
+    <row r="9" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
@@ -838,8 +865,8 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E10" s="5"/>
+    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
@@ -865,8 +892,8 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E11" s="5"/>
+    <row r="11" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
@@ -892,8 +919,8 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E12" s="5"/>
+    <row r="12" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E12" s="8"/>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
@@ -919,8 +946,8 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E13" s="5"/>
+    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
@@ -946,8 +973,8 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E14" s="5"/>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
@@ -973,24 +1000,24 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E15" s="4">
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E15" s="7">
         <v>500</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="K15" s="2">
         <v>1.02</v>
@@ -1002,8 +1029,8 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E16" s="4"/>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
       <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1029,8 +1056,8 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E17" s="4"/>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
       <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1056,8 +1083,8 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E18" s="4"/>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1083,8 +1110,8 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E19" s="4"/>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" s="7"/>
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1110,8 +1137,8 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E20" s="4"/>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E20" s="7"/>
       <c r="F20" s="2" t="s">
         <v>2</v>
       </c>
@@ -1137,8 +1164,8 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E21" s="4"/>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1164,8 +1191,8 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E22" s="4"/>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
       <c r="F22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1191,8 +1218,8 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E23" s="4"/>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E23" s="7"/>
       <c r="F23" s="2" t="s">
         <v>5</v>
       </c>
@@ -1218,8 +1245,8 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E24" s="4"/>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E24" s="7"/>
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1245,27 +1272,27 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E25" s="5">
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E25" s="8">
         <v>1000</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="J25" s="1">
         <v>1.02</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1274,8 +1301,8 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E26" s="5"/>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1301,8 +1328,8 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E27" s="5"/>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
       <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1328,8 +1355,8 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E28" s="5"/>
+    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
       <c r="F28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1355,8 +1382,8 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E29" s="5"/>
+    <row r="29" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
       <c r="F29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1382,8 +1409,8 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E30" s="5"/>
+    <row r="30" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
       <c r="F30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1409,8 +1436,8 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E31" s="5"/>
+    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E31" s="8"/>
       <c r="F31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1436,8 +1463,8 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E32" s="5"/>
+    <row r="32" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E32" s="8"/>
       <c r="F32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1463,8 +1490,8 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E33" s="5"/>
+    <row r="33" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E33" s="8"/>
       <c r="F33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1490,8 +1517,8 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E34" s="5"/>
+    <row r="34" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E34" s="8"/>
       <c r="F34" s="1" t="s">
         <v>6</v>
       </c>
@@ -1517,8 +1544,8 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E35" s="4">
+    <row r="35" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E35" s="7">
         <v>2000</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -1536,8 +1563,8 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E36" s="4"/>
+    <row r="36" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E36" s="7"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
@@ -1553,8 +1580,8 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E37" s="4"/>
+    <row r="37" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E37" s="7"/>
       <c r="F37" s="2" t="s">
         <v>10</v>
       </c>
@@ -1570,8 +1597,8 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E38" s="4"/>
+    <row r="38" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
         <v>11</v>
       </c>
@@ -1587,8 +1614,8 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E39" s="4"/>
+    <row r="39" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
       <c r="F39" s="2" t="s">
         <v>12</v>
       </c>
@@ -1604,8 +1631,8 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E40" s="4"/>
+    <row r="40" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E40" s="7"/>
       <c r="F40" s="2" t="s">
         <v>2</v>
       </c>
@@ -1621,8 +1648,8 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E41" s="4"/>
+    <row r="41" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E41" s="7"/>
       <c r="F41" s="2" t="s">
         <v>3</v>
       </c>
@@ -1638,8 +1665,8 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E42" s="4"/>
+    <row r="42" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E42" s="7"/>
       <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
@@ -1655,8 +1682,8 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E43" s="4"/>
+    <row r="43" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
       <c r="F43" s="2" t="s">
         <v>5</v>
       </c>
@@ -1672,8 +1699,8 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E44" s="4"/>
+    <row r="44" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
       <c r="F44" s="2" t="s">
         <v>6</v>
       </c>
@@ -1689,8 +1716,8 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E45" s="5">
+    <row r="45" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E45" s="8">
         <v>3000</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -1718,8 +1745,8 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E46" s="5"/>
+    <row r="46" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E46" s="8"/>
       <c r="F46" s="1" t="s">
         <v>9</v>
       </c>
@@ -1745,8 +1772,8 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E47" s="5"/>
+    <row r="47" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E47" s="8"/>
       <c r="F47" s="1" t="s">
         <v>10</v>
       </c>
@@ -1772,8 +1799,8 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E48" s="5"/>
+    <row r="48" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E48" s="8"/>
       <c r="F48" s="1" t="s">
         <v>11</v>
       </c>
@@ -1799,8 +1826,8 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E49" s="5"/>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E49" s="8"/>
       <c r="F49" s="1" t="s">
         <v>12</v>
       </c>
@@ -1826,8 +1853,8 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E50" s="5"/>
+    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E50" s="8"/>
       <c r="F50" s="1" t="s">
         <v>2</v>
       </c>
@@ -1853,8 +1880,8 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E51" s="5"/>
+    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E51" s="8"/>
       <c r="F51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1880,8 +1907,8 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E52" s="5"/>
+    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E52" s="8"/>
       <c r="F52" s="1" t="s">
         <v>4</v>
       </c>
@@ -1907,8 +1934,8 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E53" s="5"/>
+    <row r="53" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E53" s="8"/>
       <c r="F53" s="1" t="s">
         <v>5</v>
       </c>
@@ -1934,8 +1961,8 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E54" s="5"/>
+    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E54" s="8"/>
       <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
@@ -1961,8 +1988,8 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E55" s="4">
+    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E55" s="7">
         <v>4000</v>
       </c>
       <c r="F55" s="2" t="s">
@@ -1980,8 +2007,8 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E56" s="4"/>
+    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E56" s="7"/>
       <c r="F56" s="2" t="s">
         <v>9</v>
       </c>
@@ -1997,8 +2024,8 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E57" s="4"/>
+    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E57" s="7"/>
       <c r="F57" s="2" t="s">
         <v>10</v>
       </c>
@@ -2014,8 +2041,8 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E58" s="4"/>
+    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E58" s="7"/>
       <c r="F58" s="2" t="s">
         <v>11</v>
       </c>
@@ -2031,8 +2058,8 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E59" s="4"/>
+    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E59" s="7"/>
       <c r="F59" s="2" t="s">
         <v>12</v>
       </c>
@@ -2048,8 +2075,8 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E60" s="4"/>
+    <row r="60" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E60" s="7"/>
       <c r="F60" s="2" t="s">
         <v>2</v>
       </c>
@@ -2065,8 +2092,8 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E61" s="4"/>
+    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E61" s="7"/>
       <c r="F61" s="2" t="s">
         <v>3</v>
       </c>
@@ -2082,8 +2109,8 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E62" s="4"/>
+    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E62" s="7"/>
       <c r="F62" s="2" t="s">
         <v>4</v>
       </c>
@@ -2099,8 +2126,8 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E63" s="4"/>
+    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E63" s="7"/>
       <c r="F63" s="2" t="s">
         <v>5</v>
       </c>
@@ -2116,8 +2143,8 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E64" s="4"/>
+    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E64" s="7"/>
       <c r="F64" s="2" t="s">
         <v>6</v>
       </c>
@@ -2133,8 +2160,8 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E65" s="5">
+    <row r="65" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E65" s="8">
         <v>5000</v>
       </c>
       <c r="F65" s="1" t="s">
@@ -2160,8 +2187,8 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E66" s="5"/>
+    <row r="66" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E66" s="8"/>
       <c r="F66" s="1" t="s">
         <v>9</v>
       </c>
@@ -2185,8 +2212,8 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E67" s="5"/>
+    <row r="67" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E67" s="8"/>
       <c r="F67" s="1" t="s">
         <v>10</v>
       </c>
@@ -2210,8 +2237,8 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E68" s="5"/>
+    <row r="68" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E68" s="8"/>
       <c r="F68" s="1" t="s">
         <v>11</v>
       </c>
@@ -2235,8 +2262,8 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E69" s="5"/>
+    <row r="69" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E69" s="8"/>
       <c r="F69" s="1" t="s">
         <v>12</v>
       </c>
@@ -2260,8 +2287,8 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E70" s="5"/>
+    <row r="70" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E70" s="8"/>
       <c r="F70" s="1" t="s">
         <v>2</v>
       </c>
@@ -2285,8 +2312,8 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E71" s="5"/>
+    <row r="71" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E71" s="8"/>
       <c r="F71" s="1" t="s">
         <v>3</v>
       </c>
@@ -2310,8 +2337,8 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E72" s="5"/>
+    <row r="72" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E72" s="8"/>
       <c r="F72" s="1" t="s">
         <v>4</v>
       </c>
@@ -2335,8 +2362,8 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E73" s="5"/>
+    <row r="73" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E73" s="8"/>
       <c r="F73" s="1" t="s">
         <v>5</v>
       </c>
@@ -2360,8 +2387,8 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E74" s="5"/>
+    <row r="74" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E74" s="8"/>
       <c r="F74" s="1" t="s">
         <v>6</v>
       </c>
@@ -2404,36 +2431,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B69CDB-A77A-4566-B4FD-FEF3E3113682}">
   <dimension ref="E2:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="C48" workbookViewId="0">
+      <selection activeCell="Q74" sqref="Q74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="33" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="11" width="10.7265625" customWidth="1"/>
+    <col min="7" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="5" t="s">
+    <row r="2" spans="5:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="5:17" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="5:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2474,8 +2501,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E5" s="5">
+    <row r="5" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E5" s="8">
         <v>100</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -2503,25 +2530,25 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E6" s="5"/>
+    <row r="6" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E6" s="8"/>
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -2530,8 +2557,8 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E7" s="5"/>
+    <row r="7" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E7" s="8"/>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2557,8 +2584,8 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E8" s="5"/>
+    <row r="8" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E8" s="8"/>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2584,8 +2611,8 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E9" s="5"/>
+    <row r="9" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2611,8 +2638,8 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E10" s="5"/>
+    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2638,8 +2665,8 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E11" s="5"/>
+    <row r="11" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
@@ -2665,8 +2692,8 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E12" s="5"/>
+    <row r="12" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E12" s="8"/>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2692,10 +2719,10 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E13" s="5"/>
+    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1">
         <v>1.6</v>
@@ -2719,8 +2746,8 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E14" s="5"/>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2746,8 +2773,8 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E15" s="4">
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E15" s="7">
         <v>500</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2775,25 +2802,25 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E16" s="4"/>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
       <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -2802,8 +2829,8 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E17" s="4"/>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
       <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2829,8 +2856,8 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E18" s="4"/>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
         <v>11</v>
       </c>
@@ -2856,8 +2883,8 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E19" s="4"/>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" s="7"/>
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
@@ -2883,8 +2910,8 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E20" s="4"/>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E20" s="7"/>
       <c r="F20" s="2" t="s">
         <v>2</v>
       </c>
@@ -2910,8 +2937,8 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E21" s="4"/>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2937,8 +2964,8 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E22" s="4"/>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
       <c r="F22" s="2" t="s">
         <v>4</v>
       </c>
@@ -2964,10 +2991,10 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E23" s="4"/>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E23" s="7"/>
       <c r="F23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="2">
         <v>7.1</v>
@@ -2991,8 +3018,8 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E24" s="4"/>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E24" s="7"/>
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
@@ -3018,8 +3045,8 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E25" s="5">
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E25" s="8">
         <v>1000</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -3047,25 +3074,25 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E26" s="5"/>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -3074,8 +3101,8 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E27" s="5"/>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
       <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
@@ -3101,8 +3128,8 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E28" s="5"/>
+    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
       <c r="F28" s="1" t="s">
         <v>11</v>
       </c>
@@ -3128,8 +3155,8 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E29" s="5"/>
+    <row r="29" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
       <c r="F29" s="1" t="s">
         <v>12</v>
       </c>
@@ -3155,8 +3182,8 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E30" s="5"/>
+    <row r="30" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
       <c r="F30" s="1" t="s">
         <v>2</v>
       </c>
@@ -3182,8 +3209,8 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E31" s="5"/>
+    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E31" s="8"/>
       <c r="F31" s="1" t="s">
         <v>3</v>
       </c>
@@ -3209,8 +3236,8 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E32" s="5"/>
+    <row r="32" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E32" s="8"/>
       <c r="F32" s="1" t="s">
         <v>4</v>
       </c>
@@ -3236,10 +3263,10 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E33" s="5"/>
+    <row r="33" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E33" s="8"/>
       <c r="F33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" s="1">
         <v>7.7</v>
@@ -3263,8 +3290,8 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E34" s="5"/>
+    <row r="34" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E34" s="8"/>
       <c r="F34" s="1" t="s">
         <v>6</v>
       </c>
@@ -3290,8 +3317,8 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E35" s="4">
+    <row r="35" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E35" s="7">
         <v>2000</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -3309,8 +3336,8 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E36" s="4"/>
+    <row r="36" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E36" s="7"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
@@ -3326,8 +3353,8 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E37" s="4"/>
+    <row r="37" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E37" s="7"/>
       <c r="F37" s="2" t="s">
         <v>10</v>
       </c>
@@ -3343,8 +3370,8 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E38" s="4"/>
+    <row r="38" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
         <v>11</v>
       </c>
@@ -3360,8 +3387,8 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E39" s="4"/>
+    <row r="39" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
       <c r="F39" s="2" t="s">
         <v>12</v>
       </c>
@@ -3377,8 +3404,8 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E40" s="4"/>
+    <row r="40" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E40" s="7"/>
       <c r="F40" s="2" t="s">
         <v>2</v>
       </c>
@@ -3394,8 +3421,8 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E41" s="4"/>
+    <row r="41" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E41" s="7"/>
       <c r="F41" s="2" t="s">
         <v>3</v>
       </c>
@@ -3411,8 +3438,8 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E42" s="4"/>
+    <row r="42" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E42" s="7"/>
       <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
@@ -3428,10 +3455,10 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E43" s="4"/>
+    <row r="43" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
       <c r="F43" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -3445,8 +3472,8 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E44" s="4"/>
+    <row r="44" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
       <c r="F44" s="2" t="s">
         <v>6</v>
       </c>
@@ -3462,8 +3489,8 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E45" s="5">
+    <row r="45" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E45" s="8">
         <v>3000</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -3491,25 +3518,25 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E46" s="5"/>
+    <row r="46" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E46" s="8"/>
       <c r="F46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -3518,8 +3545,8 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E47" s="5"/>
+    <row r="47" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E47" s="8"/>
       <c r="F47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3545,8 +3572,8 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E48" s="5"/>
+    <row r="48" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E48" s="8"/>
       <c r="F48" s="1" t="s">
         <v>11</v>
       </c>
@@ -3572,8 +3599,8 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E49" s="5"/>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E49" s="8"/>
       <c r="F49" s="1" t="s">
         <v>12</v>
       </c>
@@ -3599,8 +3626,8 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E50" s="5"/>
+    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E50" s="8"/>
       <c r="F50" s="1" t="s">
         <v>2</v>
       </c>
@@ -3626,8 +3653,8 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E51" s="5"/>
+    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E51" s="8"/>
       <c r="F51" s="1" t="s">
         <v>3</v>
       </c>
@@ -3653,8 +3680,8 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E52" s="5"/>
+    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E52" s="8"/>
       <c r="F52" s="1" t="s">
         <v>4</v>
       </c>
@@ -3680,10 +3707,10 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E53" s="5"/>
+    <row r="53" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E53" s="8"/>
       <c r="F53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G53" s="1">
         <v>8.1</v>
@@ -3707,8 +3734,8 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E54" s="5"/>
+    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E54" s="8"/>
       <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
@@ -3734,8 +3761,8 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E55" s="4">
+    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E55" s="7">
         <v>4000</v>
       </c>
       <c r="F55" s="2" t="s">
@@ -3753,8 +3780,8 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E56" s="4"/>
+    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E56" s="7"/>
       <c r="F56" s="2" t="s">
         <v>9</v>
       </c>
@@ -3770,8 +3797,8 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E57" s="4"/>
+    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E57" s="7"/>
       <c r="F57" s="2" t="s">
         <v>10</v>
       </c>
@@ -3787,8 +3814,8 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E58" s="4"/>
+    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E58" s="7"/>
       <c r="F58" s="2" t="s">
         <v>11</v>
       </c>
@@ -3804,8 +3831,8 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E59" s="4"/>
+    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E59" s="7"/>
       <c r="F59" s="2" t="s">
         <v>12</v>
       </c>
@@ -3821,8 +3848,8 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E60" s="4"/>
+    <row r="60" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E60" s="7"/>
       <c r="F60" s="2" t="s">
         <v>2</v>
       </c>
@@ -3838,8 +3865,8 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E61" s="4"/>
+    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E61" s="7"/>
       <c r="F61" s="2" t="s">
         <v>3</v>
       </c>
@@ -3855,8 +3882,8 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E62" s="4"/>
+    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E62" s="7"/>
       <c r="F62" s="2" t="s">
         <v>4</v>
       </c>
@@ -3872,10 +3899,10 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E63" s="4"/>
+    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E63" s="7"/>
       <c r="F63" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -3889,8 +3916,8 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E64" s="4"/>
+    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E64" s="7"/>
       <c r="F64" s="2" t="s">
         <v>6</v>
       </c>
@@ -3906,8 +3933,8 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E65" s="5">
+    <row r="65" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E65" s="8">
         <v>5000</v>
       </c>
       <c r="F65" s="1" t="s">
@@ -3916,7 +3943,7 @@
       <c r="G65" s="1">
         <v>8910</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H65" s="4">
         <v>8970</v>
       </c>
       <c r="I65" s="1">
@@ -3935,25 +3962,25 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E66" s="5"/>
+    <row r="66" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E66" s="8"/>
       <c r="F66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -3962,8 +3989,8 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E67" s="5"/>
+    <row r="67" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E67" s="8"/>
       <c r="F67" s="1" t="s">
         <v>10</v>
       </c>
@@ -3989,8 +4016,8 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E68" s="5"/>
+    <row r="68" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E68" s="8"/>
       <c r="F68" s="1" t="s">
         <v>11</v>
       </c>
@@ -4016,8 +4043,8 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E69" s="5"/>
+    <row r="69" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E69" s="8"/>
       <c r="F69" s="1" t="s">
         <v>12</v>
       </c>
@@ -4043,8 +4070,8 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E70" s="5"/>
+    <row r="70" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E70" s="8"/>
       <c r="F70" s="1" t="s">
         <v>2</v>
       </c>
@@ -4070,8 +4097,8 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E71" s="5"/>
+    <row r="71" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E71" s="8"/>
       <c r="F71" s="1" t="s">
         <v>3</v>
       </c>
@@ -4097,8 +4124,8 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E72" s="5"/>
+    <row r="72" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E72" s="8"/>
       <c r="F72" s="1" t="s">
         <v>4</v>
       </c>
@@ -4124,10 +4151,10 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E73" s="5"/>
+    <row r="73" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E73" s="8"/>
       <c r="F73" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G73" s="1">
         <v>8.1</v>
@@ -4151,8 +4178,8 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E74" s="5"/>
+    <row r="74" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E74" s="8"/>
       <c r="F74" s="1" t="s">
         <v>6</v>
       </c>
@@ -4195,38 +4222,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA5084B-E471-40D4-8120-C3A0E03070E3}">
-  <dimension ref="E2:Q74"/>
+  <dimension ref="E2:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="33" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="11" width="10.7265625" customWidth="1"/>
+    <col min="7" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="5" t="s">
+    <row r="2" spans="5:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="5:17" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="5:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4267,299 +4294,359 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E5" s="5">
+    <row r="5" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E5" s="8">
         <v>100</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>3.32</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3.01</v>
+        <v>37.78</v>
+      </c>
+      <c r="H5" s="5">
+        <v>19.2</v>
       </c>
       <c r="I5" s="1">
-        <v>3.05</v>
-      </c>
-      <c r="J5" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="K5" s="1">
-        <v>3.09</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+        <v>39.54</v>
+      </c>
+      <c r="J5" s="5">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E6" s="5"/>
+    <row r="6" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E6" s="8"/>
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>47</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E7" s="5"/>
+    <row r="7" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E7" s="8"/>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="1">
-        <v>1560</v>
-      </c>
-      <c r="H7" s="1">
-        <v>170.44</v>
+        <v>464.38</v>
+      </c>
+      <c r="H7" s="5">
+        <v>307.77</v>
       </c>
       <c r="I7" s="1">
-        <v>56.23</v>
-      </c>
-      <c r="J7" s="1">
-        <v>162.9</v>
+        <v>500.38</v>
+      </c>
+      <c r="J7" s="5">
+        <v>414.42</v>
       </c>
       <c r="K7" s="1">
-        <v>160.77000000000001</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+        <v>1690</v>
+      </c>
+      <c r="L7" s="5">
+        <v>214.28</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="5">
+        <v>306.75</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E8" s="5"/>
+    <row r="8" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E8" s="8"/>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="1">
-        <v>4.26</v>
-      </c>
-      <c r="H8" s="1">
-        <v>3.57</v>
+        <v>64.89</v>
+      </c>
+      <c r="H8" s="5">
+        <v>28.82</v>
       </c>
       <c r="I8" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="J8" s="1">
-        <v>4.16</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3.98</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+        <v>58.93</v>
+      </c>
+      <c r="J8" s="5">
+        <v>28.95</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="5">
+        <v>40.92</v>
+      </c>
+      <c r="M8" s="5">
+        <v>29.59</v>
+      </c>
+      <c r="N8" s="5">
+        <v>30.02</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E9" s="5"/>
+    <row r="9" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="1">
-        <v>4.96</v>
-      </c>
-      <c r="H9" s="1">
-        <v>4.07</v>
+        <v>106.61</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="I9" s="1">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="J9" s="1">
-        <v>4.78</v>
-      </c>
-      <c r="K9" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+        <v>90.11</v>
+      </c>
+      <c r="J9" s="5">
+        <v>36.46</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="5">
+        <v>54.84</v>
+      </c>
+      <c r="M9" s="5">
+        <v>38.39</v>
+      </c>
+      <c r="N9" s="5">
+        <v>38.58</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E10" s="5"/>
+    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="1">
-        <v>83806</v>
-      </c>
-      <c r="H10" s="1">
-        <v>83830</v>
+        <v>40467</v>
+      </c>
+      <c r="H10" s="5">
+        <v>41202</v>
       </c>
       <c r="I10" s="1">
-        <v>83827</v>
-      </c>
-      <c r="J10" s="1">
-        <v>83815</v>
+        <v>40400</v>
+      </c>
+      <c r="J10" s="5">
+        <v>41199</v>
       </c>
       <c r="K10" s="1">
-        <v>83821</v>
-      </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+        <v>40040</v>
+      </c>
+      <c r="L10" s="5">
+        <v>41032</v>
+      </c>
+      <c r="M10" s="5">
+        <v>41223</v>
+      </c>
+      <c r="N10" s="5">
+        <v>41190</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E11" s="5"/>
+    <row r="11" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="1">
-        <v>960.7</v>
-      </c>
-      <c r="H11" s="1">
-        <v>960.3</v>
+        <v>481.6</v>
+      </c>
+      <c r="H11" s="5">
+        <v>480.6</v>
       </c>
       <c r="I11" s="1">
-        <v>960.3</v>
-      </c>
-      <c r="J11" s="1">
-        <v>960.3</v>
+        <v>480.8</v>
+      </c>
+      <c r="J11" s="5">
+        <v>480.5</v>
       </c>
       <c r="K11" s="1">
-        <v>960.3</v>
-      </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+        <v>480.4</v>
+      </c>
+      <c r="L11" s="5">
+        <v>480.4</v>
+      </c>
+      <c r="M11" s="5">
+        <v>480.3</v>
+      </c>
+      <c r="N11" s="5">
+        <v>480.6</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E12" s="5"/>
+    <row r="12" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E12" s="8"/>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="1">
-        <v>87.24</v>
-      </c>
-      <c r="H12" s="1">
-        <v>87.29</v>
+        <v>84.03</v>
+      </c>
+      <c r="H12" s="5">
+        <v>85.74</v>
       </c>
       <c r="I12" s="1">
-        <v>87.29</v>
-      </c>
-      <c r="J12" s="1">
-        <v>87.28</v>
+        <v>84.02</v>
+      </c>
+      <c r="J12" s="5">
+        <v>85.74</v>
       </c>
       <c r="K12" s="1">
-        <v>87.29</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+        <v>83.34</v>
+      </c>
+      <c r="L12" s="5">
+        <v>85.41</v>
+      </c>
+      <c r="M12" s="5">
+        <v>85.82</v>
+      </c>
+      <c r="N12" s="5">
+        <v>85.7</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E13" s="5"/>
+    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1">
-        <v>14</v>
-      </c>
-      <c r="H13" s="1">
-        <v>14</v>
+        <v>7.6</v>
+      </c>
+      <c r="H13" s="5">
+        <v>7.7</v>
       </c>
       <c r="I13" s="1">
-        <v>14</v>
-      </c>
-      <c r="J13" s="1">
-        <v>14</v>
+        <v>7.6</v>
+      </c>
+      <c r="J13" s="5">
+        <v>7.7</v>
       </c>
       <c r="K13" s="1">
-        <v>14</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="L13" s="5">
+        <v>7.7</v>
+      </c>
+      <c r="M13" s="5">
+        <v>7.7</v>
+      </c>
+      <c r="N13" s="5">
+        <v>7.7</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E14" s="5"/>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="1">
-        <v>8.6</v>
-      </c>
-      <c r="H14" s="1">
-        <v>8.6</v>
+        <v>25</v>
+      </c>
+      <c r="H14" s="5">
+        <v>25</v>
       </c>
       <c r="I14" s="1">
-        <v>8.6</v>
-      </c>
-      <c r="J14" s="1">
-        <v>8.6</v>
+        <v>25</v>
+      </c>
+      <c r="J14" s="5">
+        <v>25</v>
       </c>
       <c r="K14" s="1">
-        <v>8.6</v>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="L14" s="5">
+        <v>25</v>
+      </c>
+      <c r="M14" s="5">
+        <v>25</v>
+      </c>
+      <c r="N14" s="5">
+        <v>25</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E15" s="4">
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E15" s="7">
         <v>500</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="2">
-        <v>312.95</v>
+        <v>3490</v>
       </c>
       <c r="H15" s="2">
-        <v>325.12</v>
+        <v>3510</v>
       </c>
       <c r="I15" s="2">
-        <v>324.31</v>
+        <v>3480</v>
       </c>
       <c r="J15" s="2">
-        <v>332.28</v>
+        <v>3490</v>
       </c>
       <c r="K15" s="2">
-        <v>318.62</v>
+        <v>3480</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -4568,25 +4655,25 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E16" s="4"/>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
       <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -4595,25 +4682,25 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E17" s="4"/>
+    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
       <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="2">
-        <v>583.91</v>
+        <v>4840</v>
       </c>
       <c r="H17" s="2">
-        <v>597.28</v>
+        <v>4830</v>
       </c>
       <c r="I17" s="2">
-        <v>618.04</v>
+        <v>4740</v>
       </c>
       <c r="J17" s="2">
-        <v>1001</v>
+        <v>4800</v>
       </c>
       <c r="K17" s="2">
-        <v>1530</v>
+        <v>4730</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -4621,26 +4708,32 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E18" s="4"/>
+      <c r="S17" t="s">
+        <v>72</v>
+      </c>
+      <c r="T17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="2">
-        <v>370.87</v>
+        <v>4030</v>
       </c>
       <c r="H18" s="2">
-        <v>386.16</v>
+        <v>4070</v>
       </c>
       <c r="I18" s="2">
-        <v>384.93</v>
+        <v>4020</v>
       </c>
       <c r="J18" s="2">
-        <v>423.54</v>
+        <v>4020</v>
       </c>
       <c r="K18" s="2">
-        <v>387.38</v>
+        <v>4010</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -4648,26 +4741,32 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E19" s="4"/>
+      <c r="S18" t="s">
+        <v>74</v>
+      </c>
+      <c r="T18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E19" s="7"/>
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="2">
-        <v>374.37</v>
+        <v>4050</v>
       </c>
       <c r="H19" s="2">
-        <v>391.24</v>
+        <v>4080</v>
       </c>
       <c r="I19" s="2">
-        <v>388.61</v>
+        <v>4030</v>
       </c>
       <c r="J19" s="2">
-        <v>455.33</v>
+        <v>4030</v>
       </c>
       <c r="K19" s="2">
-        <v>397.05</v>
+        <v>4030</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -4676,25 +4775,25 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E20" s="4"/>
+    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E20" s="7"/>
       <c r="F20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G20" s="2">
-        <v>320053</v>
+        <v>46831</v>
       </c>
       <c r="H20" s="2">
-        <v>317115</v>
+        <v>46623</v>
       </c>
       <c r="I20" s="2">
-        <v>317305</v>
+        <v>46933</v>
       </c>
       <c r="J20" s="2">
-        <v>315407</v>
+        <v>46804</v>
       </c>
       <c r="K20" s="2">
-        <v>318676</v>
+        <v>46919</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -4703,25 +4802,25 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E21" s="4"/>
+    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="2">
-        <v>960.8</v>
+        <v>480.7</v>
       </c>
       <c r="H21" s="2">
-        <v>960.7</v>
+        <v>480.9</v>
       </c>
       <c r="I21" s="2">
-        <v>960.5</v>
+        <v>480.6</v>
       </c>
       <c r="J21" s="2">
-        <v>960.7</v>
+        <v>480.4</v>
       </c>
       <c r="K21" s="2">
-        <v>960.5</v>
+        <v>480.5</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -4730,25 +4829,25 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E22" s="4"/>
+    <row r="22" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
       <c r="F22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G22" s="2">
-        <v>333.12</v>
+        <v>97.42</v>
       </c>
       <c r="H22" s="2">
-        <v>330.1</v>
+        <v>96.95</v>
       </c>
       <c r="I22" s="2">
-        <v>330.34</v>
+        <v>97.65</v>
       </c>
       <c r="J22" s="2">
-        <v>328.32</v>
+        <v>97.42</v>
       </c>
       <c r="K22" s="2">
-        <v>331.78</v>
+        <v>97.64</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -4757,25 +4856,25 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E23" s="4"/>
+    <row r="23" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E23" s="7"/>
       <c r="F23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="2">
-        <v>53</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H23" s="2">
-        <v>53</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I23" s="2">
-        <v>53</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J23" s="2">
-        <v>53</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K23" s="2">
-        <v>53</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -4784,25 +4883,25 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E24" s="4"/>
+    <row r="24" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E24" s="7"/>
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H24" s="2">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I24" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J24" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K24" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -4811,27 +4910,27 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E25" s="5">
+    <row r="25" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E25" s="8">
         <v>1000</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="1">
-        <v>1500</v>
+        <v>7980</v>
       </c>
       <c r="H25" s="1">
-        <v>1480</v>
+        <v>7910</v>
       </c>
       <c r="I25" s="1">
-        <v>1480</v>
+        <v>8010</v>
       </c>
       <c r="J25" s="1">
-        <v>1560</v>
+        <v>7920</v>
       </c>
       <c r="K25" s="1">
-        <v>1490</v>
+        <v>7940</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -4840,25 +4939,25 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E26" s="5"/>
+    <row r="26" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1.03</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1.1399999999999999</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -4867,25 +4966,25 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E27" s="5"/>
+    <row r="27" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
       <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="1">
-        <v>2010</v>
+        <v>10010</v>
       </c>
       <c r="H27" s="1">
-        <v>1900</v>
+        <v>9770</v>
       </c>
       <c r="I27" s="1">
-        <v>1970</v>
+        <v>9910</v>
       </c>
       <c r="J27" s="1">
-        <v>2370</v>
+        <v>9700</v>
       </c>
       <c r="K27" s="1">
-        <v>2170</v>
+        <v>9870</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -4894,25 +4993,25 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E28" s="5"/>
+    <row r="28" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
       <c r="F28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="1">
-        <v>1740</v>
+        <v>9140</v>
       </c>
       <c r="H28" s="1">
-        <v>1710</v>
+        <v>9050</v>
       </c>
       <c r="I28" s="1">
-        <v>1720</v>
+        <v>9190</v>
       </c>
       <c r="J28" s="1">
-        <v>1990</v>
+        <v>9080</v>
       </c>
       <c r="K28" s="1">
-        <v>1740</v>
+        <v>9080</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -4921,25 +5020,25 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E29" s="5"/>
+    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
       <c r="F29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="1">
-        <v>1790</v>
+        <v>9190</v>
       </c>
       <c r="H29" s="1">
-        <v>1720</v>
+        <v>9060</v>
       </c>
       <c r="I29" s="1">
-        <v>1720</v>
+        <v>9220</v>
       </c>
       <c r="J29" s="1">
-        <v>2020</v>
+        <v>9110</v>
       </c>
       <c r="K29" s="1">
-        <v>1790</v>
+        <v>9120</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -4948,25 +5047,25 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E30" s="5"/>
+    <row r="30" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
       <c r="F30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G30" s="1">
-        <v>167918</v>
+        <v>47058</v>
       </c>
       <c r="H30" s="1">
-        <v>169521</v>
+        <v>47391</v>
       </c>
       <c r="I30" s="1">
-        <v>169309</v>
+        <v>46911</v>
       </c>
       <c r="J30" s="1">
-        <v>163726</v>
+        <v>47363</v>
       </c>
       <c r="K30" s="1">
-        <v>168616</v>
+        <v>47260</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -4975,25 +5074,25 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E31" s="5"/>
+    <row r="31" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E31" s="8"/>
       <c r="F31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="1">
+        <v>480.6</v>
+      </c>
+      <c r="H31" s="1">
         <v>480.8</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
+        <v>480.8</v>
+      </c>
+      <c r="J31" s="1">
+        <v>480.9</v>
+      </c>
+      <c r="K31" s="1">
         <v>481</v>
-      </c>
-      <c r="I31" s="1">
-        <v>480.5</v>
-      </c>
-      <c r="J31" s="1">
-        <v>480.7</v>
-      </c>
-      <c r="K31" s="1">
-        <v>480.5</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -5002,25 +5101,25 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E32" s="5"/>
+    <row r="32" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E32" s="8"/>
       <c r="F32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="1">
-        <v>349.23</v>
+        <v>97.91</v>
       </c>
       <c r="H32" s="1">
-        <v>352.46</v>
+        <v>98.57</v>
       </c>
       <c r="I32" s="1">
-        <v>352.34</v>
+        <v>97.56</v>
       </c>
       <c r="J32" s="1">
-        <v>340.57</v>
+        <v>98.49</v>
       </c>
       <c r="K32" s="1">
-        <v>350.89</v>
+        <v>98.25</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -5029,25 +5128,25 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E33" s="5"/>
+    <row r="33" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E33" s="8"/>
       <c r="F33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" s="1">
-        <v>28</v>
+        <v>8.9</v>
       </c>
       <c r="H33" s="1">
-        <v>28</v>
+        <v>8.9</v>
       </c>
       <c r="I33" s="1">
-        <v>28</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J33" s="1">
-        <v>27</v>
+        <v>8.9</v>
       </c>
       <c r="K33" s="1">
-        <v>28</v>
+        <v>8.9</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -5056,25 +5155,25 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E34" s="5"/>
+    <row r="34" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E34" s="8"/>
       <c r="F34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G34" s="1">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H34" s="1">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I34" s="1">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J34" s="1">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="K34" s="1">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -5083,28 +5182,18 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E35" s="4">
+    <row r="35" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E35" s="7">
         <v>2000</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G35" s="2">
-        <v>3880</v>
-      </c>
-      <c r="H35" s="2">
-        <v>3830</v>
-      </c>
-      <c r="I35" s="2">
-        <v>3840</v>
-      </c>
-      <c r="J35" s="2">
-        <v>3870</v>
-      </c>
-      <c r="K35" s="2">
-        <v>4360</v>
-      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5112,26 +5201,16 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E36" s="4"/>
+    <row r="36" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E36" s="7"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5139,26 +5218,16 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E37" s="4"/>
+    <row r="37" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E37" s="7"/>
       <c r="F37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="2">
-        <v>4690</v>
-      </c>
-      <c r="H37" s="2">
-        <v>4650</v>
-      </c>
-      <c r="I37" s="2">
-        <v>4610</v>
-      </c>
-      <c r="J37" s="2">
-        <v>4650</v>
-      </c>
-      <c r="K37" s="2">
-        <v>5190</v>
-      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5166,26 +5235,16 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E38" s="4"/>
+    <row r="38" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="2">
-        <v>4450</v>
-      </c>
-      <c r="H38" s="2">
-        <v>4410</v>
-      </c>
-      <c r="I38" s="2">
-        <v>4410</v>
-      </c>
-      <c r="J38" s="2">
-        <v>4450</v>
-      </c>
-      <c r="K38" s="2">
-        <v>4980</v>
-      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5193,26 +5252,16 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E39" s="4"/>
+    <row r="39" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
       <c r="F39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="2">
-        <v>4490</v>
-      </c>
-      <c r="H39" s="2">
-        <v>4430</v>
-      </c>
-      <c r="I39" s="2">
-        <v>4430</v>
-      </c>
-      <c r="J39" s="2">
-        <v>4460</v>
-      </c>
-      <c r="K39" s="2">
-        <v>4990</v>
-      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5220,26 +5269,16 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E40" s="4"/>
+    <row r="40" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E40" s="7"/>
       <c r="F40" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="2">
-        <v>172730</v>
-      </c>
-      <c r="H40" s="2">
-        <v>174395</v>
-      </c>
-      <c r="I40" s="2">
-        <v>174050</v>
-      </c>
-      <c r="J40" s="2">
-        <v>172746</v>
-      </c>
-      <c r="K40" s="2">
-        <v>157175</v>
-      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5247,26 +5286,16 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E41" s="4"/>
+    <row r="41" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E41" s="7"/>
       <c r="F41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="2">
-        <v>480.6</v>
-      </c>
-      <c r="H41" s="2">
-        <v>480.6</v>
-      </c>
-      <c r="I41" s="2">
-        <v>480.7</v>
-      </c>
-      <c r="J41" s="2">
-        <v>480.6</v>
-      </c>
-      <c r="K41" s="2">
-        <v>480.7</v>
-      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5274,26 +5303,16 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E42" s="4"/>
+    <row r="42" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E42" s="7"/>
       <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="2">
-        <v>359.38</v>
-      </c>
-      <c r="H42" s="2">
-        <v>362.86</v>
-      </c>
-      <c r="I42" s="2">
-        <v>362.08</v>
-      </c>
-      <c r="J42" s="2">
-        <v>359.42</v>
-      </c>
-      <c r="K42" s="2">
-        <v>326.97000000000003</v>
-      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5301,26 +5320,16 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E43" s="4"/>
+    <row r="43" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
       <c r="F43" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="2">
-        <v>29</v>
-      </c>
-      <c r="H43" s="2">
-        <v>29</v>
-      </c>
-      <c r="I43" s="2">
-        <v>29</v>
-      </c>
-      <c r="J43" s="2">
-        <v>29</v>
-      </c>
-      <c r="K43" s="2">
-        <v>26</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5328,26 +5337,16 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E44" s="4"/>
+    <row r="44" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
       <c r="F44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="2">
-        <v>18</v>
-      </c>
-      <c r="H44" s="2">
-        <v>18</v>
-      </c>
-      <c r="I44" s="2">
-        <v>18</v>
-      </c>
-      <c r="J44" s="2">
-        <v>18</v>
-      </c>
-      <c r="K44" s="2">
-        <v>16</v>
-      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5355,28 +5354,24 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E45" s="5">
+    <row r="45" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
         <v>3000</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G45" s="1">
-        <v>6510</v>
+        <v>25310</v>
       </c>
       <c r="H45" s="1">
-        <v>6330</v>
+        <v>25260</v>
       </c>
       <c r="I45" s="1">
-        <v>6380</v>
-      </c>
-      <c r="J45" s="1">
-        <v>6340</v>
-      </c>
-      <c r="K45" s="1">
-        <v>6280</v>
-      </c>
+        <v>20270</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -5384,26 +5379,20 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E46" s="5"/>
+    <row r="46" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="H46" s="1">
+        <v>3.19</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -5411,26 +5400,20 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E47" s="5"/>
+    <row r="47" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G47" s="1">
-        <v>7640</v>
+      <c r="G47">
+        <v>33830</v>
       </c>
       <c r="H47" s="1">
-        <v>7440</v>
-      </c>
-      <c r="I47" s="1">
-        <v>7540</v>
-      </c>
-      <c r="J47" s="1">
-        <v>7470</v>
-      </c>
-      <c r="K47" s="1">
-        <v>7380</v>
-      </c>
+        <v>29950</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
@@ -5438,26 +5421,20 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E48" s="5"/>
+    <row r="48" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="1">
-        <v>7480</v>
-      </c>
-      <c r="H48" s="1">
-        <v>7250</v>
-      </c>
-      <c r="I48" s="1">
-        <v>7330</v>
-      </c>
-      <c r="J48" s="1">
-        <v>7260</v>
-      </c>
-      <c r="K48" s="1">
-        <v>7180</v>
-      </c>
+        <v>33070</v>
+      </c>
+      <c r="H48" s="6">
+        <v>29250</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
@@ -5465,26 +5442,20 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E49" s="5"/>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G49" s="1">
-        <v>7510</v>
+        <v>33280</v>
       </c>
       <c r="H49" s="1">
-        <v>7270</v>
-      </c>
-      <c r="I49" s="1">
-        <v>7350</v>
-      </c>
-      <c r="J49" s="1">
-        <v>7280</v>
-      </c>
-      <c r="K49" s="1">
-        <v>7200</v>
-      </c>
+        <v>29300</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
@@ -5492,26 +5463,20 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E50" s="5"/>
+    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E50" s="9"/>
       <c r="F50" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G50" s="1">
-        <v>168681</v>
+        <v>55845</v>
       </c>
       <c r="H50" s="1">
-        <v>172603</v>
-      </c>
-      <c r="I50" s="1">
-        <v>171644</v>
-      </c>
-      <c r="J50" s="1">
-        <v>172365</v>
-      </c>
-      <c r="K50" s="1">
-        <v>173853</v>
-      </c>
+        <v>83282</v>
+      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
@@ -5519,26 +5484,20 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E51" s="5"/>
+    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E51" s="9"/>
       <c r="F51" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G51" s="1">
-        <v>480.9</v>
+        <v>6001</v>
       </c>
       <c r="H51" s="1">
-        <v>480.9</v>
-      </c>
-      <c r="I51" s="1">
-        <v>480.8</v>
-      </c>
-      <c r="J51" s="1">
-        <v>480.7</v>
-      </c>
-      <c r="K51" s="1">
-        <v>480.9</v>
-      </c>
+        <v>840.5</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
@@ -5546,26 +5505,20 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E52" s="5"/>
+    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E52" s="9"/>
       <c r="F52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G52" s="1">
-        <v>350.8</v>
+        <v>552.79</v>
       </c>
       <c r="H52" s="1">
-        <v>359.14</v>
-      </c>
-      <c r="I52" s="1">
-        <v>356.98</v>
-      </c>
-      <c r="J52" s="1">
-        <v>358.59</v>
-      </c>
-      <c r="K52" s="1">
-        <v>361.54</v>
-      </c>
+        <v>99.08</v>
+      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
@@ -5573,26 +5526,20 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E53" s="5"/>
+    <row r="53" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E53" s="9"/>
       <c r="F53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G53" s="1">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H53" s="1">
-        <v>29</v>
-      </c>
-      <c r="I53" s="1">
-        <v>29</v>
-      </c>
-      <c r="J53" s="1">
-        <v>29</v>
-      </c>
-      <c r="K53" s="1">
-        <v>29</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
@@ -5600,26 +5547,20 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E54" s="5"/>
+    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E54" s="10"/>
       <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G54" s="1">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H54" s="1">
-        <v>18</v>
-      </c>
-      <c r="I54" s="1">
-        <v>18</v>
-      </c>
-      <c r="J54" s="1">
-        <v>18</v>
-      </c>
-      <c r="K54" s="1">
-        <v>18</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -5627,28 +5568,18 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E55" s="4">
+    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E55" s="7">
         <v>4000</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G55" s="2">
-        <v>8800</v>
-      </c>
-      <c r="H55" s="2">
-        <v>8850</v>
-      </c>
-      <c r="I55" s="2">
-        <v>9060</v>
-      </c>
-      <c r="J55" s="2">
-        <v>8750</v>
-      </c>
-      <c r="K55" s="2">
-        <v>8710</v>
-      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -5656,26 +5587,16 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E56" s="4"/>
+    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E56" s="7"/>
       <c r="F56" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -5683,26 +5604,16 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E57" s="4"/>
+    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E57" s="7"/>
       <c r="F57" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G57" s="2">
-        <v>11320</v>
-      </c>
-      <c r="H57" s="2">
-        <v>10560</v>
-      </c>
-      <c r="I57" s="2">
-        <v>11110</v>
-      </c>
-      <c r="J57" s="2">
-        <v>10220</v>
-      </c>
-      <c r="K57" s="2">
-        <v>10370</v>
-      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -5710,26 +5621,16 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E58" s="4"/>
+    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E58" s="7"/>
       <c r="F58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G58" s="2">
-        <v>10220</v>
-      </c>
-      <c r="H58" s="2">
-        <v>10290</v>
-      </c>
-      <c r="I58" s="2">
-        <v>10910</v>
-      </c>
-      <c r="J58" s="2">
-        <v>9990</v>
-      </c>
-      <c r="K58" s="2">
-        <v>9970</v>
-      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -5737,26 +5638,16 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E59" s="4"/>
+    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E59" s="7"/>
       <c r="F59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="2">
-        <v>10410</v>
-      </c>
-      <c r="H59" s="2">
-        <v>10340</v>
-      </c>
-      <c r="I59" s="2">
-        <v>10930</v>
-      </c>
-      <c r="J59" s="2">
-        <v>10000</v>
-      </c>
-      <c r="K59" s="2">
-        <v>9990</v>
-      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -5764,26 +5655,16 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E60" s="4"/>
+    <row r="60" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E60" s="7"/>
       <c r="F60" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G60" s="2">
-        <v>172529</v>
-      </c>
-      <c r="H60" s="2">
-        <v>171738</v>
-      </c>
-      <c r="I60" s="2">
-        <v>168163</v>
-      </c>
-      <c r="J60" s="2">
-        <v>173529</v>
-      </c>
-      <c r="K60" s="2">
-        <v>174311</v>
-      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -5791,26 +5672,16 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E61" s="4"/>
+    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E61" s="7"/>
       <c r="F61" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G61" s="2">
-        <v>480.9</v>
-      </c>
-      <c r="H61" s="2">
-        <v>480.5</v>
-      </c>
-      <c r="I61" s="2">
-        <v>480.7</v>
-      </c>
-      <c r="J61" s="2">
-        <v>480.7</v>
-      </c>
-      <c r="K61" s="2">
-        <v>480.6</v>
-      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -5818,26 +5689,16 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E62" s="4"/>
+    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E62" s="7"/>
       <c r="F62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="2">
-        <v>358.78</v>
-      </c>
-      <c r="H62" s="2">
-        <v>357.42</v>
-      </c>
-      <c r="I62" s="2">
-        <v>349.85</v>
-      </c>
-      <c r="J62" s="2">
-        <v>361</v>
-      </c>
-      <c r="K62" s="2">
-        <v>362.7</v>
-      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -5845,26 +5706,16 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E63" s="4"/>
+    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E63" s="7"/>
       <c r="F63" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" s="2">
-        <v>29</v>
-      </c>
-      <c r="H63" s="2">
-        <v>29</v>
-      </c>
-      <c r="I63" s="2">
-        <v>28</v>
-      </c>
-      <c r="J63" s="2">
-        <v>29</v>
-      </c>
-      <c r="K63" s="2">
-        <v>29</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -5872,26 +5723,16 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E64" s="4"/>
+    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E64" s="7"/>
       <c r="F64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="2">
-        <v>18</v>
-      </c>
-      <c r="H64" s="2">
-        <v>18</v>
-      </c>
-      <c r="I64" s="2">
-        <v>17</v>
-      </c>
-      <c r="J64" s="2">
-        <v>18</v>
-      </c>
-      <c r="K64" s="2">
-        <v>18</v>
-      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -5899,28 +5740,18 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E65" s="5">
+    <row r="65" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E65" s="8">
         <v>5000</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G65" s="1">
-        <v>11500</v>
-      </c>
-      <c r="H65" s="1">
-        <v>11800</v>
-      </c>
-      <c r="I65" s="1">
-        <v>11650</v>
-      </c>
-      <c r="J65" s="1">
-        <v>11230</v>
-      </c>
-      <c r="K65" s="1">
-        <v>11400</v>
-      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
@@ -5928,26 +5759,16 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E66" s="5"/>
+    <row r="66" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E66" s="8"/>
       <c r="F66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H66" t="s">
-        <v>25</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
@@ -5955,26 +5776,16 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E67" s="5"/>
+    <row r="67" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E67" s="8"/>
       <c r="F67" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G67" s="1">
-        <v>65000</v>
-      </c>
-      <c r="H67" s="1">
-        <v>14280</v>
-      </c>
-      <c r="I67" s="1">
-        <v>71000</v>
-      </c>
-      <c r="J67" s="1">
-        <v>14800</v>
-      </c>
-      <c r="K67" s="1">
-        <v>13280</v>
-      </c>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
@@ -5982,26 +5793,16 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E68" s="5"/>
+    <row r="68" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E68" s="8"/>
       <c r="F68" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G68" s="1">
-        <v>12930</v>
-      </c>
-      <c r="H68" s="1">
-        <v>13520</v>
-      </c>
-      <c r="I68" s="1">
-        <v>13030</v>
-      </c>
-      <c r="J68" s="1">
-        <v>13200</v>
-      </c>
-      <c r="K68" s="1">
-        <v>13000</v>
-      </c>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
@@ -6009,26 +5810,16 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E69" s="5"/>
+    <row r="69" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E69" s="8"/>
       <c r="F69" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G69" s="1">
-        <v>12980</v>
-      </c>
-      <c r="H69" s="1">
-        <v>13630</v>
-      </c>
-      <c r="I69" s="1">
-        <v>13150</v>
-      </c>
-      <c r="J69" s="1">
-        <v>13220</v>
-      </c>
-      <c r="K69" s="1">
-        <v>13020</v>
-      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
@@ -6036,26 +5827,16 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E70" s="5"/>
+    <row r="70" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E70" s="8"/>
       <c r="F70" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G70" s="1">
-        <v>335230</v>
-      </c>
-      <c r="H70" s="1">
-        <v>323091</v>
-      </c>
-      <c r="I70" s="1">
-        <v>330530</v>
-      </c>
-      <c r="J70" s="1">
-        <v>173208</v>
-      </c>
-      <c r="K70" s="1">
-        <v>170963</v>
-      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -6063,26 +5844,16 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E71" s="5"/>
+    <row r="71" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E71" s="8"/>
       <c r="F71" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G71" s="1">
-        <v>990.1</v>
-      </c>
-      <c r="H71" s="1">
-        <v>1002.3</v>
-      </c>
-      <c r="I71" s="1">
-        <v>989.8</v>
-      </c>
-      <c r="J71" s="1">
-        <v>480.9</v>
-      </c>
-      <c r="K71" s="1">
-        <v>480.8</v>
-      </c>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
@@ -6090,26 +5861,16 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E72" s="5"/>
+    <row r="72" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E72" s="8"/>
       <c r="F72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G72" s="1">
-        <v>338.69</v>
-      </c>
-      <c r="H72" s="1">
-        <v>322.35000000000002</v>
-      </c>
-      <c r="I72" s="1">
-        <v>333.95</v>
-      </c>
-      <c r="J72" s="1">
-        <v>360.14</v>
-      </c>
-      <c r="K72" s="1">
-        <v>355.59</v>
-      </c>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
@@ -6117,26 +5878,16 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E73" s="5"/>
+    <row r="73" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E73" s="8"/>
       <c r="F73" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G73" s="1">
-        <v>56</v>
-      </c>
-      <c r="H73" s="1">
-        <v>54</v>
-      </c>
-      <c r="I73" s="1">
-        <v>55</v>
-      </c>
-      <c r="J73" s="1">
-        <v>29</v>
-      </c>
-      <c r="K73" s="1">
-        <v>29</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
@@ -6144,26 +5895,16 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="E74" s="5"/>
+    <row r="74" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E74" s="8"/>
       <c r="F74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="1">
-        <v>35</v>
-      </c>
-      <c r="H74" s="1">
-        <v>34</v>
-      </c>
-      <c r="I74" s="1">
-        <v>34</v>
-      </c>
-      <c r="J74" s="1">
-        <v>18</v>
-      </c>
-      <c r="K74" s="1">
-        <v>18</v>
-      </c>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>

</xml_diff>